<commit_message>
add test and contest files
</commit_message>
<xml_diff>
--- a/assets/benchmark.xlsx
+++ b/assets/benchmark.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katshun/dev/miniml_compiler/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F5FE912-5D94-2F4E-85E9-87A441C5AE2B}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FCBD9EF-9F0C-1146-AA9D-C24279A13A07}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11580" yWindow="5460" windowWidth="28040" windowHeight="17440" xr2:uid="{49EE3DC5-30C8-AA4B-9CAE-F905FE6C1531}"/>
+    <workbookView xWindow="760" yWindow="560" windowWidth="28040" windowHeight="17440" xr2:uid="{49EE3DC5-30C8-AA4B-9CAE-F905FE6C1531}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>C opt</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>fact</t>
+  </si>
+  <si>
+    <t>benchmark</t>
   </si>
 </sst>
 </file>
@@ -816,22 +819,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>2.99E-4</c:v>
+                  <c:v>2.0799999999999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.5799999999999998E-4</c:v>
+                  <c:v>2.1100000000000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.225E-4</c:v>
+                  <c:v>1.35885E-4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.2750000000000001E-4</c:v>
+                  <c:v>1.1661400000000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.4916699999999999E-4</c:v>
+                  <c:v>1.13125E-4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.24144E-4</c:v>
+                  <c:v>1.12656E-4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3060,6 +3063,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -3130,22 +3136,22 @@
         <v>8</v>
       </c>
       <c r="B4">
-        <v>2.99E-4</v>
+        <v>2.0799999999999999E-4</v>
       </c>
       <c r="C4">
-        <v>2.5799999999999998E-4</v>
+        <v>2.1100000000000001E-4</v>
       </c>
       <c r="D4">
-        <v>1.225E-4</v>
+        <v>1.35885E-4</v>
       </c>
       <c r="E4">
-        <v>1.2750000000000001E-4</v>
+        <v>1.1661400000000001E-4</v>
       </c>
       <c r="F4">
-        <v>1.4916699999999999E-4</v>
+        <v>1.13125E-4</v>
       </c>
       <c r="G4">
-        <v>1.24144E-4</v>
+        <v>1.12656E-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>